<commit_message>
fix bug all data di pagination master data
</commit_message>
<xml_diff>
--- a/public/Export_Suplier.xlsx
+++ b/public/Export_Suplier.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
   <si>
     <t>NAMA</t>
   </si>
@@ -32,103 +32,205 @@
     <t>UNIT</t>
   </si>
   <si>
-    <t>Ratih Titin Prastuti</t>
-  </si>
-  <si>
-    <t>non</t>
-  </si>
-  <si>
-    <t>Yayasan Agustina Tamba</t>
-  </si>
-  <si>
-    <t>KILO</t>
-  </si>
-  <si>
-    <t>Pranata Mandala</t>
-  </si>
-  <si>
-    <t>ad</t>
-  </si>
-  <si>
-    <t>Perum Wijayanti Tbk</t>
-  </si>
-  <si>
-    <t>Rafi Jefri Haryanto S.Pt</t>
-  </si>
-  <si>
-    <t>quia</t>
-  </si>
-  <si>
-    <t>PD Hartati Novitasari</t>
-  </si>
-  <si>
-    <t>PCS</t>
-  </si>
-  <si>
-    <t>Gasti Yulianti</t>
-  </si>
-  <si>
-    <t>et</t>
-  </si>
-  <si>
-    <t>PD Prasetya Hardiansyah (Persero) Tbk</t>
-  </si>
-  <si>
-    <t>Puspa Rahimah</t>
-  </si>
-  <si>
-    <t>eum</t>
-  </si>
-  <si>
-    <t>PT Siregar Manullang Tbk</t>
-  </si>
-  <si>
-    <t>Karna Jamil Prasasta</t>
-  </si>
-  <si>
-    <t>sequi</t>
-  </si>
-  <si>
-    <t>PT Haryanto (Persero) Tbk</t>
-  </si>
-  <si>
-    <t>Maimunah Hasanah M.Pd</t>
-  </si>
-  <si>
-    <t>ut</t>
-  </si>
-  <si>
-    <t>Perum Wahyudin Haryanti Tbk</t>
-  </si>
-  <si>
-    <t>Langgeng Hutasoit M.Pd</t>
-  </si>
-  <si>
-    <t>dolor</t>
-  </si>
-  <si>
-    <t>Perum Suryatmi Saefullah</t>
-  </si>
-  <si>
-    <t>BOX</t>
-  </si>
-  <si>
-    <t>Jamil Salahudin M.Farm</t>
-  </si>
-  <si>
-    <t>hic</t>
-  </si>
-  <si>
-    <t>Perum Laksmiwati</t>
-  </si>
-  <si>
-    <t>Kenzie Adiarja Marpaung</t>
-  </si>
-  <si>
-    <t>sunt</t>
-  </si>
-  <si>
-    <t>UD Budiman</t>
+    <t>adna sentral niaga</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>AMARTA</t>
+  </si>
+  <si>
+    <t>ARIS (AJM)</t>
+  </si>
+  <si>
+    <t>biskitop</t>
+  </si>
+  <si>
+    <t>CV.ABC SEJAHTERA</t>
+  </si>
+  <si>
+    <t>CV.AMC (JOMBANG)</t>
+  </si>
+  <si>
+    <t>CV.ANGKASA LEATHER</t>
+  </si>
+  <si>
+    <t>CV.BOROBUDUR PRIMA SEJAHTERA</t>
+  </si>
+  <si>
+    <t>cv.glory star indonesia</t>
+  </si>
+  <si>
+    <t>CV.INDO SINAR SURYA</t>
+  </si>
+  <si>
+    <t>cv.segoro kidul</t>
+  </si>
+  <si>
+    <t>CV.SINAR MATAHARI</t>
+  </si>
+  <si>
+    <t>cv.tiga anugerah pangan</t>
+  </si>
+  <si>
+    <t>DAMARUS</t>
+  </si>
+  <si>
+    <t>GALUH</t>
+  </si>
+  <si>
+    <t>HBM PERMEN</t>
+  </si>
+  <si>
+    <t>iboga distribution</t>
+  </si>
+  <si>
+    <t>KANCIL</t>
+  </si>
+  <si>
+    <t>MAJU JAYA(SPN)</t>
+  </si>
+  <si>
+    <t>MARTINI</t>
+  </si>
+  <si>
+    <t>mentari pelangi</t>
+  </si>
+  <si>
+    <t>MJ (MAKMUR JAYA)</t>
+  </si>
+  <si>
+    <t>MJA</t>
+  </si>
+  <si>
+    <t>MY FOOD(MIMO)</t>
+  </si>
+  <si>
+    <t>pabrik kembang gula/pasuruan</t>
+  </si>
+  <si>
+    <t>pt trisumber lintas nusantara</t>
+  </si>
+  <si>
+    <t>PT.ABADI NIAGA PRIMA</t>
+  </si>
+  <si>
+    <t>PT.ARTA BOGA CEMERLANG</t>
+  </si>
+  <si>
+    <t>PT.BERKAT KARYA LESTARI</t>
+  </si>
+  <si>
+    <t>PT.BINA SAN PRIMA</t>
+  </si>
+  <si>
+    <t>PT.CNS (CIPTA NIAGA SEMESTA)</t>
+  </si>
+  <si>
+    <t>PT.GLOBAL NARA SADHANA</t>
+  </si>
+  <si>
+    <t>pt.gonusa prima distribusi</t>
+  </si>
+  <si>
+    <t>PT.JATIM TETAP JAYA</t>
+  </si>
+  <si>
+    <t>PT.KHINGGUAN</t>
+  </si>
+  <si>
+    <t>PT.MANOHARA ADIKA DISTRINDO</t>
+  </si>
+  <si>
+    <t>PT.MITRA MENTARI JAYA PERSADA</t>
+  </si>
+  <si>
+    <t>PT.MITRA USAHA SUKSES SEJAHTERA</t>
+  </si>
+  <si>
+    <t>PT.MSD(MITRA SEJATI DISTRIBUSI)</t>
+  </si>
+  <si>
+    <t>PT.MURNI ANUGRAH MANDIRI</t>
+  </si>
+  <si>
+    <t>PT.PANDAAN LOTUS MANUFACTURE</t>
+  </si>
+  <si>
+    <t>PT.PINUS MERAH ABADI</t>
+  </si>
+  <si>
+    <t>PT.PUJI SURYA INDAH</t>
+  </si>
+  <si>
+    <t>PT.RAMASURYA PERKASA DISTRINDO</t>
+  </si>
+  <si>
+    <t>PT.SAERAH SURYA PERKASA</t>
+  </si>
+  <si>
+    <t>PT.SINAR NIAGA SEJAHTERA</t>
+  </si>
+  <si>
+    <t>PT.SINAR USAHA NIAGA</t>
+  </si>
+  <si>
+    <t>PT.SO GOOD FOOD</t>
+  </si>
+  <si>
+    <t>PT.TRI SUMBER LINTAS NUSANTARA</t>
+  </si>
+  <si>
+    <t>PT.ULTRA JAYA MILK</t>
+  </si>
+  <si>
+    <t>PT.USAHA SEJATI JAYA(USJ)</t>
+  </si>
+  <si>
+    <t>SANTOSO</t>
+  </si>
+  <si>
+    <t>SHANGHAI PANDA</t>
+  </si>
+  <si>
+    <t>SIDOARJO SURYA GEMILANG</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>SUNY BOY MALANG</t>
+  </si>
+  <si>
+    <t>TEH HIJAU</t>
+  </si>
+  <si>
+    <t>TERA ARTHA PERDANA</t>
+  </si>
+  <si>
+    <t>TK.SUMBER REJEKI/SEPANJANG</t>
+  </si>
+  <si>
+    <t>TOKO M2M/CIK NIEK</t>
+  </si>
+  <si>
+    <t>UD.BOROBUDUR PUTRA MANDIRI</t>
+  </si>
+  <si>
+    <t>UD.KUDA EMAS BERLIAN</t>
+  </si>
+  <si>
+    <t>UD.SINAR SERAYU</t>
+  </si>
+  <si>
+    <t>WILIAM RELAXA</t>
+  </si>
+  <si>
+    <t>WONG NDESO</t>
+  </si>
+  <si>
+    <t>YUDI JOMBANG</t>
   </si>
 </sst>
 </file>
@@ -498,10 +600,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -531,166 +633,1118 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2">
-        <v>739</v>
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="2">
-        <v>439</v>
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2">
-        <v>777</v>
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="2">
-        <v>865</v>
+        <v>6</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="2">
-        <v>841</v>
+        <v>6</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="2">
-        <v>201</v>
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="2">
-        <v>685</v>
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2">
-        <v>444</v>
+        <v>6</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="B34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2">
-        <v>293</v>
+      <c r="B35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>